<commit_message>
Updated Product backlog for tuesday
Added new user stories and updated status of previous ones
</commit_message>
<xml_diff>
--- a/Product_Backlog/Backlog.xlsx
+++ b/Product_Backlog/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>the website can access the data entries in the database</t>
+  </si>
+  <si>
+    <t>see markers with different colours based on price</t>
+  </si>
+  <si>
+    <t>I can visually understand the price of different locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see a visual highlight of the corresponding facility when I click on a marker </t>
+  </si>
+  <si>
+    <t>I can read what cell in the table corresponds to the marker</t>
+  </si>
+  <si>
+    <t>Click on a facility name and have it behave like clicking a marker</t>
+  </si>
+  <si>
+    <t>I can navigate the website easier</t>
   </si>
 </sst>
 </file>
@@ -229,8 +247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I21" totalsRowShown="0">
-  <autoFilter ref="A1:I21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0">
+  <autoFilter ref="A1:I24"/>
   <sortState ref="A2:I20">
     <sortCondition ref="A1:A21"/>
   </sortState>
@@ -546,17 +564,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
@@ -616,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -775,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -801,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -827,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -853,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -879,7 +897,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -957,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,7 +1001,7 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1090,6 +1108,84 @@
       </c>
       <c r="I20" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1102,21 +1198,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000A45299412FDFE49916D3B2BC7498215" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="528d0d9d29f55c94d322eb3857adfb37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7b8fda29-18fb-4238-bb7d-7bcb176bce57" xmlns:ns4="c00e3565-1744-4d61-af64-fc54f2252c20" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8027d906c71b20e95020a61b0ffa4a2b" ns3:_="" ns4:_="">
     <xsd:import namespace="7b8fda29-18fb-4238-bb7d-7bcb176bce57"/>
@@ -1307,24 +1388,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8883EC-248E-4ECC-89D3-154C0362A1E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6119A8-CD1D-4A1F-8289-F6D1316969F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD3DC6FD-6E27-4089-8EC8-B7D737193740}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1341,4 +1420,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E6119A8-CD1D-4A1F-8289-F6D1316969F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8883EC-248E-4ECC-89D3-154C0362A1E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>